<commit_message>
Modify 20 test cases
</commit_message>
<xml_diff>
--- a/d41d8cd9 (1).xlsx
+++ b/d41d8cd9 (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRI\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bonus-SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89ED0ED-BF1D-4CFA-B2C3-B9D0BC735A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67DFD3B-4490-4524-AD57-782E3CBF35A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>Sign_in_Pass</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>FeedBack</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>paas</t>
   </si>
 </sst>
 </file>
@@ -529,7 +535,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,7 +796,9 @@
       <c r="C21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -802,7 +810,9 @@
       <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -814,7 +824,9 @@
       <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -826,6 +838,9 @@
       <c r="C24" t="s">
         <v>36</v>
       </c>
+      <c r="D24" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -834,6 +849,9 @@
       <c r="B25" t="s">
         <v>39</v>
       </c>
+      <c r="D25" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -844,6 +862,9 @@
       </c>
       <c r="C26" t="s">
         <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -853,6 +874,9 @@
       <c r="B27" t="s">
         <v>40</v>
       </c>
+      <c r="D27" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -861,6 +885,9 @@
       <c r="B28" t="s">
         <v>41</v>
       </c>
+      <c r="D28" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -869,6 +896,9 @@
       <c r="B29" t="s">
         <v>43</v>
       </c>
+      <c r="D29" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -877,6 +907,9 @@
       <c r="B30" t="s">
         <v>42</v>
       </c>
+      <c r="D30" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -885,6 +918,9 @@
       <c r="B31" t="s">
         <v>44</v>
       </c>
+      <c r="D31" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -893,69 +929,96 @@
       <c r="B32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D37" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D38" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>53</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 19 test cases
</commit_message>
<xml_diff>
--- a/d41d8cd9 (1).xlsx
+++ b/d41d8cd9 (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bonus-SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67DFD3B-4490-4524-AD57-782E3CBF35A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7DA379-526E-4A9A-B9B5-5EA3555E8780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>Sign_in_Pass</t>
   </si>
@@ -193,6 +193,27 @@
   </si>
   <si>
     <t>paas</t>
+  </si>
+  <si>
+    <t>ChangeLanguage</t>
+  </si>
+  <si>
+    <t>SubmitDebugLogs</t>
+  </si>
+  <si>
+    <t>InvalidSecurityKey</t>
+  </si>
+  <si>
+    <t>SignOutThroughSetting</t>
+  </si>
+  <si>
+    <t>ChangeLanguageInSigninPage</t>
+  </si>
+  <si>
+    <t>ExploreRoomInFirstPage</t>
+  </si>
+  <si>
+    <t>CreateAccountBacktoSignInPage</t>
   </si>
 </sst>
 </file>
@@ -532,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,6 +1042,62 @@
         <v>54</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E8:E13"/>

</xml_diff>

<commit_message>
Alo Tris nho pull ve
</commit_message>
<xml_diff>
--- a/d41d8cd9 (1).xlsx
+++ b/d41d8cd9 (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bonus-SE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pikachu\Documents\Bonus-SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7DA379-526E-4A9A-B9B5-5EA3555E8780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7F9166-2934-425A-9ACC-63B023A5F2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Sign_in_Pass</t>
   </si>
@@ -114,9 +114,6 @@
     <t>nó bị chuyển sang sign up</t>
   </si>
   <si>
-    <t>:)) t hk hiểu sao cả 6 cái bị lỗi, hình như là hk tìm dc room</t>
-  </si>
-  <si>
     <t>Chuyển qua dark-&gt;Chuyển lại light</t>
   </si>
   <si>
@@ -189,12 +186,6 @@
     <t>FeedBack</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>paas</t>
-  </si>
-  <si>
     <t>ChangeLanguage</t>
   </si>
   <si>
@@ -214,6 +205,45 @@
   </si>
   <si>
     <t>CreateAccountBacktoSignInPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ChangeLanguageInWelcomePage</t>
+  </si>
+  <si>
+    <t>LogInFail</t>
+  </si>
+  <si>
+    <t>LogInByGGAccount</t>
+  </si>
+  <si>
+    <t>ChangeRoomName</t>
+  </si>
+  <si>
+    <t>PrivateToPublic</t>
+  </si>
+  <si>
+    <t>InvitePeopleToRoom</t>
+  </si>
+  <si>
+    <t>ShareLinkToUser</t>
+  </si>
+  <si>
+    <t>ShareLink</t>
+  </si>
+  <si>
+    <t>SeeFilkeInRoom</t>
+  </si>
+  <si>
+    <t>ExportChat</t>
+  </si>
+  <si>
+    <t>AdvancedInRoomSetting</t>
+  </si>
+  <si>
+    <t>SearchInRoom</t>
   </si>
 </sst>
 </file>
@@ -242,12 +272,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -262,16 +298,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,21 +596,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.21875" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.77734375" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -578,43 +621,43 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -624,11 +667,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -638,11 +681,11 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -650,10 +693,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -663,11 +706,9 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -677,9 +718,9 @@
       <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -689,9 +730,9 @@
       <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -701,9 +742,9 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -713,9 +754,9 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -725,9 +766,9 @@
       <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -738,7 +779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -749,7 +790,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -760,7 +801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -771,7 +812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -782,7 +823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -793,316 +834,473 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
       <c r="D26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
       <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
         <v>62</v>
       </c>
+      <c r="D49" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E8:E13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tri pull ve nhe duoc 46 roi
</commit_message>
<xml_diff>
--- a/d41d8cd9 (1).xlsx
+++ b/d41d8cd9 (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pikachu\Documents\Bonus-SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7F9166-2934-425A-9ACC-63B023A5F2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7DBEFF-FF83-4CA2-B5A9-C31D485DDB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="72">
   <si>
     <t>Sign_in_Pass</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>CreateAccountBacktoSignInPage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>ChangeLanguageInWelcomePage</t>
@@ -298,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -316,6 +313,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1163,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
         <v>26</v>
@@ -1176,7 +1174,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>25</v>
@@ -1187,7 +1185,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" t="s">
         <v>26</v>
@@ -1198,7 +1196,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>25</v>
@@ -1209,7 +1207,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>25</v>
@@ -1220,10 +1218,10 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1231,7 +1229,10 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,7 +1240,10 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1247,7 +1251,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,7 +1262,10 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1263,7 +1273,10 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1271,32 +1284,186 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>60</v>
       </c>
+      <c r="D60" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>61</v>
       </c>
+      <c r="D61" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62</v>
       </c>
+      <c r="D62" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
       </c>
+      <c r="D63" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>64</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="D66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="D68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="D70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="D72" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="D74" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="D75" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="D77" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="D78" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="D80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>